<commit_message>
update Dicc y WBS
</commit_message>
<xml_diff>
--- a/Diccionario.xlsx
+++ b/Diccionario.xlsx
@@ -1,13 +1,8 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="19029"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9302"/>
   <workbookPr defaultThemeVersion="124226"/>
-  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-    <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\JASHO\Desktop\DAJAYA\"/>
-    </mc:Choice>
-  </mc:AlternateContent>
   <bookViews>
     <workbookView xWindow="240" yWindow="60" windowWidth="20115" windowHeight="8010"/>
   </bookViews>
@@ -21,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="160" uniqueCount="73">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="174" uniqueCount="75">
   <si>
     <r>
       <t xml:space="preserve">Fecha de cracion: </t>
@@ -275,13 +270,19 @@
     <t>DATE</t>
   </si>
   <si>
-    <t>AUTO_INCREMENT</t>
+    <t>EXTRA</t>
+  </si>
+  <si>
+    <t>auto_increment</t>
+  </si>
+  <si>
+    <t>ASIENTO</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -333,7 +334,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="10">
+  <borders count="12">
     <border>
       <left/>
       <right/>
@@ -458,11 +459,37 @@
       <bottom/>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="21">
+  <cellXfs count="22">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
@@ -513,7 +540,10 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="11" xfId="0" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -523,9 +553,6 @@
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
       <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
-    </ext>
-    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{9260A510-F301-46a8-8635-F512D64BE5F5}">
-      <x15:timelineStyles defaultTimelineStyle="TimeSlicerStyleLight1"/>
     </ext>
   </extLst>
 </styleSheet>
@@ -574,7 +601,7 @@
     </a:clrScheme>
     <a:fontScheme name="Office">
       <a:majorFont>
-        <a:latin typeface="Cambria" panose="020F0302020204030204"/>
+        <a:latin typeface="Cambria"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -607,26 +634,9 @@
         <a:font script="Viet" typeface="Times New Roman"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
         <a:font script="Geor" typeface="Sylfaen"/>
-        <a:font script="Armn" typeface="Arial"/>
-        <a:font script="Bugi" typeface="Leelawadee UI"/>
-        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
-        <a:font script="Java" typeface="Javanese Text"/>
-        <a:font script="Lisu" typeface="Segoe UI"/>
-        <a:font script="Mymr" typeface="Myanmar Text"/>
-        <a:font script="Nkoo" typeface="Ebrima"/>
-        <a:font script="Olck" typeface="Nirmala UI"/>
-        <a:font script="Osma" typeface="Ebrima"/>
-        <a:font script="Phag" typeface="Phagspa"/>
-        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
-        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
-        <a:font script="Syre" typeface="Estrangelo Edessa"/>
-        <a:font script="Sora" typeface="Nirmala UI"/>
-        <a:font script="Tale" typeface="Microsoft Tai Le"/>
-        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
-        <a:font script="Tfng" typeface="Ebrima"/>
       </a:majorFont>
       <a:minorFont>
-        <a:latin typeface="Calibri" panose="020F0502020204030204"/>
+        <a:latin typeface="Calibri"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -659,23 +669,6 @@
         <a:font script="Viet" typeface="Arial"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
         <a:font script="Geor" typeface="Sylfaen"/>
-        <a:font script="Armn" typeface="Arial"/>
-        <a:font script="Bugi" typeface="Leelawadee UI"/>
-        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
-        <a:font script="Java" typeface="Javanese Text"/>
-        <a:font script="Lisu" typeface="Segoe UI"/>
-        <a:font script="Mymr" typeface="Myanmar Text"/>
-        <a:font script="Nkoo" typeface="Ebrima"/>
-        <a:font script="Olck" typeface="Nirmala UI"/>
-        <a:font script="Osma" typeface="Ebrima"/>
-        <a:font script="Phag" typeface="Phagspa"/>
-        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
-        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
-        <a:font script="Syre" typeface="Estrangelo Edessa"/>
-        <a:font script="Sora" typeface="Nirmala UI"/>
-        <a:font script="Tale" typeface="Microsoft Tai Le"/>
-        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
-        <a:font script="Tfng" typeface="Ebrima"/>
       </a:minorFont>
     </a:fontScheme>
     <a:fmtScheme name="Office">
@@ -852,10 +845,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:G38"/>
+  <dimension ref="A1:H37"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A2" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
-      <selection activeCell="F24" sqref="F24"/>
+    <sheetView tabSelected="1" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
+      <selection activeCell="F37" sqref="F37"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -863,26 +856,29 @@
     <col min="1" max="1" width="17" customWidth="1"/>
     <col min="2" max="2" width="13.5703125" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="16.28515625" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="31.140625" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="16.28515625" customWidth="1"/>
+    <col min="7" max="7" width="31.140625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:8" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A1" s="8"/>
       <c r="B1" s="15"/>
       <c r="C1" s="15"/>
       <c r="D1" s="15"/>
       <c r="E1" s="15"/>
       <c r="F1" s="15"/>
-    </row>
-    <row r="2" spans="1:7" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="G1" s="15"/>
+    </row>
+    <row r="2" spans="1:8" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A2" s="14"/>
       <c r="B2" s="14"/>
       <c r="C2" s="14"/>
       <c r="D2" s="14"/>
       <c r="E2" s="14"/>
       <c r="F2" s="14"/>
-    </row>
-    <row r="3" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="G2" s="14"/>
+    </row>
+    <row r="3" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A3" s="3" t="s">
         <v>36</v>
       </c>
@@ -898,11 +894,14 @@
       <c r="E3" s="4" t="s">
         <v>40</v>
       </c>
-      <c r="F3" s="5" t="s">
+      <c r="F3" s="20" t="s">
+        <v>72</v>
+      </c>
+      <c r="G3" s="5" t="s">
         <v>41</v>
       </c>
     </row>
-    <row r="4" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A4" s="12" t="s">
         <v>49</v>
       </c>
@@ -912,13 +911,16 @@
       <c r="C4" s="6" t="s">
         <v>48</v>
       </c>
-      <c r="D4" s="6"/>
+      <c r="D4" s="6">
+        <v>5</v>
+      </c>
       <c r="E4" s="6" t="s">
         <v>52</v>
       </c>
-      <c r="F4" s="7"/>
-    </row>
-    <row r="5" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="F4" s="21"/>
+      <c r="G4" s="7"/>
+    </row>
+    <row r="5" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A5" s="13"/>
       <c r="B5" s="6" t="s">
         <v>45</v>
@@ -926,13 +928,16 @@
       <c r="C5" s="6" t="s">
         <v>50</v>
       </c>
-      <c r="D5" s="6"/>
+      <c r="D5" s="6">
+        <v>30</v>
+      </c>
       <c r="E5" s="6" t="s">
         <v>42</v>
       </c>
-      <c r="F5" s="7"/>
-    </row>
-    <row r="6" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="F5" s="21"/>
+      <c r="G5" s="7"/>
+    </row>
+    <row r="6" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A6" s="13"/>
       <c r="B6" s="6" t="s">
         <v>44</v>
@@ -940,20 +945,24 @@
       <c r="C6" s="6" t="s">
         <v>46</v>
       </c>
-      <c r="D6" s="6"/>
+      <c r="D6" s="6">
+        <v>5</v>
+      </c>
       <c r="E6" s="6" t="s">
         <v>51</v>
       </c>
-      <c r="F6" s="20"/>
-    </row>
-    <row r="7" spans="1:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="F6" s="21"/>
+      <c r="G6" s="7"/>
+    </row>
+    <row r="7" spans="1:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A7" s="10"/>
       <c r="B7" s="11"/>
       <c r="C7" s="11"/>
       <c r="D7" s="11"/>
       <c r="E7" s="11"/>
-    </row>
-    <row r="8" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="F7" s="11"/>
+    </row>
+    <row r="8" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A8" s="3" t="s">
         <v>36</v>
       </c>
@@ -969,11 +978,14 @@
       <c r="E8" s="4" t="s">
         <v>40</v>
       </c>
-      <c r="F8" s="5" t="s">
+      <c r="F8" s="20" t="s">
+        <v>72</v>
+      </c>
+      <c r="G8" s="5" t="s">
         <v>41</v>
       </c>
     </row>
-    <row r="9" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A9" s="12" t="s">
         <v>43</v>
       </c>
@@ -983,15 +995,18 @@
       <c r="C9" s="6" t="s">
         <v>46</v>
       </c>
-      <c r="D9" s="6"/>
+      <c r="D9" s="6">
+        <v>5</v>
+      </c>
       <c r="E9" s="6" t="s">
         <v>42</v>
       </c>
-      <c r="F9" s="7" t="s">
-        <v>72</v>
-      </c>
-    </row>
-    <row r="10" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="F9" s="21" t="s">
+        <v>73</v>
+      </c>
+      <c r="G9" s="7"/>
+    </row>
+    <row r="10" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A10" s="13"/>
       <c r="B10" s="6" t="s">
         <v>54</v>
@@ -999,13 +1014,16 @@
       <c r="C10" s="6" t="s">
         <v>50</v>
       </c>
-      <c r="D10" s="6"/>
+      <c r="D10" s="6">
+        <v>25</v>
+      </c>
       <c r="E10" s="6" t="s">
         <v>52</v>
       </c>
-      <c r="F10" s="7"/>
-    </row>
-    <row r="11" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="F10" s="21"/>
+      <c r="G10" s="7"/>
+    </row>
+    <row r="11" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A11" s="13"/>
       <c r="B11" s="6" t="s">
         <v>45</v>
@@ -1013,13 +1031,16 @@
       <c r="C11" s="6" t="s">
         <v>50</v>
       </c>
-      <c r="D11" s="6"/>
+      <c r="D11" s="6">
+        <v>30</v>
+      </c>
       <c r="E11" s="6" t="s">
         <v>51</v>
       </c>
-      <c r="F11" s="7"/>
-    </row>
-    <row r="12" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="F11" s="21"/>
+      <c r="G11" s="7"/>
+    </row>
+    <row r="12" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A12" s="13"/>
       <c r="B12" s="6" t="s">
         <v>55</v>
@@ -1027,13 +1048,16 @@
       <c r="C12" s="6" t="s">
         <v>50</v>
       </c>
-      <c r="D12" s="6"/>
+      <c r="D12" s="6">
+        <v>10</v>
+      </c>
       <c r="E12" s="6" t="s">
         <v>52</v>
       </c>
-      <c r="F12" s="7"/>
-    </row>
-    <row r="13" spans="1:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="F12" s="21"/>
+      <c r="G12" s="7"/>
+    </row>
+    <row r="13" spans="1:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A13" s="10"/>
       <c r="B13" s="11"/>
       <c r="C13" s="11"/>
@@ -1041,8 +1065,9 @@
       <c r="E13" s="11"/>
       <c r="F13" s="11"/>
       <c r="G13" s="11"/>
-    </row>
-    <row r="14" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="H13" s="11"/>
+    </row>
+    <row r="14" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A14" s="3" t="s">
         <v>36</v>
       </c>
@@ -1058,12 +1083,15 @@
       <c r="E14" s="4" t="s">
         <v>40</v>
       </c>
-      <c r="F14" s="5" t="s">
+      <c r="F14" s="20" t="s">
+        <v>72</v>
+      </c>
+      <c r="G14" s="5" t="s">
         <v>41</v>
       </c>
-      <c r="G14" s="11"/>
-    </row>
-    <row r="15" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="H14" s="11"/>
+    </row>
+    <row r="15" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A15" s="12" t="s">
         <v>62</v>
       </c>
@@ -1073,14 +1101,19 @@
       <c r="C15" s="6" t="s">
         <v>46</v>
       </c>
-      <c r="D15" s="6"/>
+      <c r="D15" s="6">
+        <v>5</v>
+      </c>
       <c r="E15" s="6" t="s">
         <v>42</v>
       </c>
-      <c r="F15" s="7"/>
-      <c r="G15" s="11"/>
-    </row>
-    <row r="16" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="F15" s="21" t="s">
+        <v>73</v>
+      </c>
+      <c r="G15" s="7"/>
+      <c r="H15" s="11"/>
+    </row>
+    <row r="16" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A16" s="13"/>
       <c r="B16" s="6" t="s">
         <v>59</v>
@@ -1088,14 +1121,19 @@
       <c r="C16" s="6" t="s">
         <v>46</v>
       </c>
-      <c r="D16" s="6"/>
+      <c r="D16" s="6">
+        <v>5</v>
+      </c>
       <c r="E16" s="6" t="s">
-        <v>52</v>
-      </c>
-      <c r="F16" s="7"/>
-      <c r="G16" s="11"/>
-    </row>
-    <row r="17" spans="1:7" x14ac:dyDescent="0.25">
+        <v>42</v>
+      </c>
+      <c r="F16" s="21" t="s">
+        <v>73</v>
+      </c>
+      <c r="G16" s="7"/>
+      <c r="H16" s="11"/>
+    </row>
+    <row r="17" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A17" s="13"/>
       <c r="B17" s="6" t="s">
         <v>56</v>
@@ -1103,14 +1141,17 @@
       <c r="C17" s="6" t="s">
         <v>50</v>
       </c>
-      <c r="D17" s="6"/>
+      <c r="D17" s="6">
+        <v>8</v>
+      </c>
       <c r="E17" s="6" t="s">
         <v>51</v>
       </c>
-      <c r="F17" s="7"/>
-      <c r="G17" s="11"/>
-    </row>
-    <row r="18" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="F17" s="21"/>
+      <c r="G17" s="7"/>
+      <c r="H17" s="11"/>
+    </row>
+    <row r="18" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A18" s="13"/>
       <c r="B18" s="6" t="s">
         <v>57</v>
@@ -1118,14 +1159,17 @@
       <c r="C18" s="6" t="s">
         <v>50</v>
       </c>
-      <c r="D18" s="6"/>
+      <c r="D18" s="6">
+        <v>25</v>
+      </c>
       <c r="E18" s="6" t="s">
         <v>52</v>
       </c>
-      <c r="F18" s="7"/>
-      <c r="G18" s="11"/>
-    </row>
-    <row r="19" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="F18" s="21"/>
+      <c r="G18" s="7"/>
+      <c r="H18" s="11"/>
+    </row>
+    <row r="19" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A19" s="9"/>
       <c r="B19" s="6" t="s">
         <v>58</v>
@@ -1133,13 +1177,18 @@
       <c r="C19" s="6" t="s">
         <v>50</v>
       </c>
-      <c r="D19" s="6"/>
-      <c r="E19" s="6"/>
+      <c r="D19" s="6">
+        <v>25</v>
+      </c>
+      <c r="E19" s="6" t="s">
+        <v>52</v>
+      </c>
       <c r="F19" s="6"/>
-      <c r="G19" s="11"/>
-    </row>
-    <row r="20" spans="1:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
-    <row r="21" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="G19" s="6"/>
+      <c r="H19" s="11"/>
+    </row>
+    <row r="20" spans="1:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
+    <row r="21" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A21" s="3" t="s">
         <v>36</v>
       </c>
@@ -1155,11 +1204,14 @@
       <c r="E21" s="4" t="s">
         <v>40</v>
       </c>
-      <c r="F21" s="5" t="s">
+      <c r="F21" s="20" t="s">
+        <v>72</v>
+      </c>
+      <c r="G21" s="5" t="s">
         <v>41</v>
       </c>
     </row>
-    <row r="22" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A22" s="12" t="s">
         <v>60</v>
       </c>
@@ -1169,15 +1221,18 @@
       <c r="C22" s="6" t="s">
         <v>46</v>
       </c>
-      <c r="D22" s="6"/>
+      <c r="D22" s="6">
+        <v>5</v>
+      </c>
       <c r="E22" s="6" t="s">
         <v>42</v>
       </c>
-      <c r="F22" s="7" t="s">
-        <v>72</v>
-      </c>
-    </row>
-    <row r="23" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="F22" s="21" t="s">
+        <v>73</v>
+      </c>
+      <c r="G22" s="7"/>
+    </row>
+    <row r="23" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A23" s="13"/>
       <c r="B23" s="6" t="s">
         <v>54</v>
@@ -1185,13 +1240,16 @@
       <c r="C23" s="6" t="s">
         <v>50</v>
       </c>
-      <c r="D23" s="6"/>
+      <c r="D23" s="6">
+        <v>25</v>
+      </c>
       <c r="E23" s="6" t="s">
         <v>52</v>
       </c>
-      <c r="F23" s="7"/>
-    </row>
-    <row r="24" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="F23" s="21"/>
+      <c r="G23" s="7"/>
+    </row>
+    <row r="24" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A24" s="13"/>
       <c r="B24" s="6" t="s">
         <v>63</v>
@@ -1199,13 +1257,16 @@
       <c r="C24" s="6" t="s">
         <v>50</v>
       </c>
-      <c r="D24" s="6"/>
+      <c r="D24" s="6">
+        <v>30</v>
+      </c>
       <c r="E24" s="6" t="s">
         <v>52</v>
       </c>
-      <c r="F24" s="7"/>
-    </row>
-    <row r="25" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="F24" s="21"/>
+      <c r="G24" s="7"/>
+    </row>
+    <row r="25" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A25" s="13"/>
       <c r="B25" s="6" t="s">
         <v>64</v>
@@ -1213,14 +1274,17 @@
       <c r="C25" s="6" t="s">
         <v>50</v>
       </c>
-      <c r="D25" s="6"/>
+      <c r="D25" s="6">
+        <v>20</v>
+      </c>
       <c r="E25" s="6" t="s">
         <v>52</v>
       </c>
-      <c r="F25" s="7"/>
-    </row>
-    <row r="26" spans="1:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
-    <row r="27" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="F25" s="21"/>
+      <c r="G25" s="7"/>
+    </row>
+    <row r="26" spans="1:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
+    <row r="27" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A27" s="3" t="s">
         <v>36</v>
       </c>
@@ -1236,11 +1300,14 @@
       <c r="E27" s="4" t="s">
         <v>40</v>
       </c>
-      <c r="F27" s="5" t="s">
+      <c r="F27" s="20" t="s">
+        <v>72</v>
+      </c>
+      <c r="G27" s="5" t="s">
         <v>41</v>
       </c>
     </row>
-    <row r="28" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A28" s="12" t="s">
         <v>65</v>
       </c>
@@ -1250,142 +1317,171 @@
       <c r="C28" s="6" t="s">
         <v>46</v>
       </c>
-      <c r="D28" s="6"/>
+      <c r="D28" s="6">
+        <v>5</v>
+      </c>
       <c r="E28" s="6" t="s">
         <v>42</v>
       </c>
-      <c r="F28" s="7" t="s">
+      <c r="F28" s="21" t="s">
+        <v>73</v>
+      </c>
+      <c r="G28" s="7"/>
+    </row>
+    <row r="29" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A29" s="13"/>
+      <c r="B29" s="6" t="s">
+        <v>53</v>
+      </c>
+      <c r="C29" s="6" t="s">
+        <v>46</v>
+      </c>
+      <c r="D29" s="6">
+        <v>5</v>
+      </c>
+      <c r="E29" s="6" t="s">
+        <v>51</v>
+      </c>
+      <c r="F29" s="21"/>
+      <c r="G29" s="7"/>
+    </row>
+    <row r="30" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A30" s="13"/>
+      <c r="B30" s="6" t="s">
+        <v>74</v>
+      </c>
+      <c r="C30" s="6" t="s">
+        <v>50</v>
+      </c>
+      <c r="D30" s="6">
+        <v>5</v>
+      </c>
+      <c r="E30" s="6" t="s">
+        <v>52</v>
+      </c>
+      <c r="F30" s="21"/>
+      <c r="G30" s="7"/>
+    </row>
+    <row r="31" spans="1:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
+    <row r="32" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A32" s="3" t="s">
+        <v>36</v>
+      </c>
+      <c r="B32" s="4" t="s">
+        <v>37</v>
+      </c>
+      <c r="C32" s="4" t="s">
+        <v>38</v>
+      </c>
+      <c r="D32" s="4" t="s">
+        <v>39</v>
+      </c>
+      <c r="E32" s="4" t="s">
+        <v>40</v>
+      </c>
+      <c r="F32" s="20" t="s">
         <v>72</v>
       </c>
-    </row>
-    <row r="29" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A29" s="13"/>
-      <c r="B29" s="6"/>
-      <c r="C29" s="6"/>
-      <c r="D29" s="6"/>
-      <c r="E29" s="6"/>
-      <c r="F29" s="7"/>
-    </row>
-    <row r="30" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A30" s="13"/>
-      <c r="B30" s="6"/>
-      <c r="C30" s="6"/>
-      <c r="D30" s="6"/>
-      <c r="E30" s="6"/>
-      <c r="F30" s="7"/>
-    </row>
-    <row r="31" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A31" s="13"/>
-      <c r="B31" s="6"/>
-      <c r="C31" s="6"/>
-      <c r="D31" s="6"/>
-      <c r="E31" s="6"/>
-      <c r="F31" s="7"/>
-    </row>
-    <row r="32" spans="1:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
-    <row r="33" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A33" s="3" t="s">
-        <v>36</v>
-      </c>
-      <c r="B33" s="4" t="s">
-        <v>37</v>
-      </c>
-      <c r="C33" s="4" t="s">
-        <v>38</v>
-      </c>
-      <c r="D33" s="4" t="s">
-        <v>39</v>
-      </c>
-      <c r="E33" s="4" t="s">
-        <v>40</v>
-      </c>
-      <c r="F33" s="5" t="s">
+      <c r="G32" s="5" t="s">
         <v>41</v>
       </c>
     </row>
-    <row r="34" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A34" s="12" t="s">
+    <row r="33" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A33" s="12" t="s">
         <v>68</v>
       </c>
+      <c r="B33" s="6" t="s">
+        <v>67</v>
+      </c>
+      <c r="C33" s="6" t="s">
+        <v>46</v>
+      </c>
+      <c r="D33" s="6">
+        <v>5</v>
+      </c>
+      <c r="E33" s="6" t="s">
+        <v>42</v>
+      </c>
+      <c r="F33" s="21" t="s">
+        <v>73</v>
+      </c>
+      <c r="G33" s="7"/>
+    </row>
+    <row r="34" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A34" s="13"/>
       <c r="B34" s="6" t="s">
-        <v>67</v>
+        <v>70</v>
       </c>
       <c r="C34" s="6" t="s">
-        <v>46</v>
-      </c>
-      <c r="D34" s="6"/>
+        <v>71</v>
+      </c>
+      <c r="D34" s="6">
+        <v>12</v>
+      </c>
       <c r="E34" s="6" t="s">
-        <v>42</v>
-      </c>
-      <c r="F34" s="7" t="s">
-        <v>72</v>
-      </c>
-    </row>
-    <row r="35" spans="1:6" x14ac:dyDescent="0.25">
+        <v>52</v>
+      </c>
+      <c r="F34" s="21"/>
+      <c r="G34" s="7"/>
+    </row>
+    <row r="35" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A35" s="13"/>
       <c r="B35" s="6" t="s">
-        <v>70</v>
+        <v>53</v>
       </c>
       <c r="C35" s="6" t="s">
-        <v>71</v>
-      </c>
-      <c r="D35" s="6"/>
+        <v>46</v>
+      </c>
+      <c r="D35" s="6">
+        <v>5</v>
+      </c>
       <c r="E35" s="6" t="s">
-        <v>52</v>
-      </c>
-      <c r="F35" s="7"/>
-    </row>
-    <row r="36" spans="1:6" x14ac:dyDescent="0.25">
+        <v>51</v>
+      </c>
+      <c r="F35" s="21"/>
+      <c r="G35" s="7"/>
+    </row>
+    <row r="36" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A36" s="13"/>
       <c r="B36" s="6" t="s">
-        <v>53</v>
+        <v>45</v>
       </c>
       <c r="C36" s="6" t="s">
-        <v>46</v>
-      </c>
-      <c r="D36" s="6"/>
+        <v>50</v>
+      </c>
+      <c r="D36" s="6">
+        <v>30</v>
+      </c>
       <c r="E36" s="6" t="s">
         <v>51</v>
       </c>
-      <c r="F36" s="7" t="s">
-        <v>72</v>
-      </c>
-    </row>
-    <row r="37" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="F36" s="21"/>
+      <c r="G36" s="7"/>
+    </row>
+    <row r="37" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A37" s="13"/>
       <c r="B37" s="6" t="s">
-        <v>45</v>
+        <v>69</v>
       </c>
       <c r="C37" s="6" t="s">
-        <v>50</v>
-      </c>
-      <c r="D37" s="6"/>
+        <v>46</v>
+      </c>
+      <c r="D37" s="6">
+        <v>5</v>
+      </c>
       <c r="E37" s="6" t="s">
-        <v>51</v>
-      </c>
-      <c r="F37" s="7"/>
-    </row>
-    <row r="38" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A38" s="13"/>
-      <c r="B38" s="6" t="s">
-        <v>69</v>
-      </c>
-      <c r="C38" s="6" t="s">
-        <v>46</v>
-      </c>
-      <c r="D38" s="6"/>
-      <c r="E38" s="6" t="s">
         <v>52</v>
       </c>
-      <c r="F38" s="7"/>
+      <c r="F37" s="21"/>
+      <c r="G37" s="7"/>
     </row>
   </sheetData>
   <mergeCells count="8">
-    <mergeCell ref="A2:F2"/>
-    <mergeCell ref="B1:F1"/>
+    <mergeCell ref="A2:G2"/>
+    <mergeCell ref="B1:G1"/>
     <mergeCell ref="A22:A25"/>
-    <mergeCell ref="A28:A31"/>
-    <mergeCell ref="A34:A38"/>
+    <mergeCell ref="A28:A30"/>
+    <mergeCell ref="A33:A37"/>
     <mergeCell ref="A9:A12"/>
     <mergeCell ref="A4:A6"/>
     <mergeCell ref="A15:A18"/>

</xml_diff>